<commit_message>
add checks to format_input
</commit_message>
<xml_diff>
--- a/input_files.xlsx
+++ b/input_files.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukefunk/packages/NatureProtocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1075D9F-FC5B-6846-B076-4A7E8FADEAFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9107370-030D-0146-BFF1-B6AE001372BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>original filename</t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>input_sbs/raw/10X_c4_B3_DAPI_Site-0.tif</t>
+  </si>
+  <si>
+    <t>DAPI</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -363,7 +378,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -419,8 +434,8 @@
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4">
-        <v>3</v>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="H2" s="5" t="str">
         <f>"input/"&amp;B2&amp;"_c"&amp;C2&amp;"-SBS-"&amp;C2&amp;"/"&amp;B2&amp;"_c"&amp;C2&amp;"-SBS-"&amp;C2&amp;"_Tile-"&amp;E2&amp;"."&amp;F2&amp;".tif"</f>
@@ -446,8 +461,8 @@
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4">
-        <v>2</v>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="H3" s="5" t="str">
         <f>"input/"&amp;B3&amp;"_c"&amp;C3&amp;"-SBS-"&amp;C3&amp;"/"&amp;B3&amp;"_c"&amp;C3&amp;"-SBS-"&amp;C3&amp;"_Tile-"&amp;E3&amp;"."&amp;F3&amp;".tif"</f>
@@ -473,8 +488,8 @@
       <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4">
-        <v>4</v>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H4" s="5" t="str">
         <f>"input/"&amp;B4&amp;"_c"&amp;C4&amp;"-SBS-"&amp;C4&amp;"/"&amp;B4&amp;"_c"&amp;C4&amp;"-SBS-"&amp;C4&amp;"_Tile-"&amp;E4&amp;"."&amp;F4&amp;".tif"</f>
@@ -500,8 +515,8 @@
       <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="4">
-        <v>5</v>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H5" s="5" t="str">
         <f>"input/"&amp;B5&amp;"_c"&amp;C5&amp;"-SBS-"&amp;C5&amp;"/"&amp;B5&amp;"_c"&amp;C5&amp;"-SBS-"&amp;C5&amp;"_Tile-"&amp;E5&amp;"."&amp;F5&amp;".tif"</f>
@@ -527,8 +542,8 @@
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="4">
-        <v>1</v>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="H6" s="5" t="str">
         <f>"input/"&amp;B6&amp;"_c"&amp;C6&amp;"-SBS-"&amp;C6&amp;"/"&amp;B6&amp;"_c"&amp;C6&amp;"-SBS-"&amp;C6&amp;"_Tile-"&amp;E6&amp;"."&amp;F6&amp;".tif"</f>

</xml_diff>